<commit_message>
changed app name from sdmf to handuflow
</commit_message>
<xml_diff>
--- a/files_dev/master_specs.xlsx
+++ b/files_dev/master_specs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hando\dev2\sdmf-official\files_dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE9C54-3C25-4993-BBED-7C16A3B53966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AABC138-25C9-4E48-9A7C-AF8241693C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="209" xr2:uid="{9E3D2F59-A0F5-48A1-B731-1D8811F4785E}"/>
   </bookViews>
@@ -1104,7 +1104,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>